<commit_message>
Added part of the code that generates the weight column.
</commit_message>
<xml_diff>
--- a/model/GDP_SDMX_Model.xlsx
+++ b/model/GDP_SDMX_Model.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAP\Fiji\sdd-fbs-data-portal-data-preparation\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71C0B395-112C-4252-B9A8-AD9F52429DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E20B9FE-A779-43F8-BFA1-A5AE991CBD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSD" sheetId="1" r:id="rId1"/>
     <sheet name="INDICATOR" sheetId="7" r:id="rId2"/>
-    <sheet name="GDP_TYPE" sheetId="10" r:id="rId3"/>
+    <sheet name="TRANSFORMATION" sheetId="10" r:id="rId3"/>
     <sheet name="INDUSTRY_TYPE" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
   <si>
     <t>Concepts</t>
   </si>
@@ -191,12 +191,6 @@
     <t>data source</t>
   </si>
   <si>
-    <t>FJD</t>
-  </si>
-  <si>
-    <t>Amount in Fiji Dollar</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -257,12 +251,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>Percentage Change</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
     <t>Gross Value Added</t>
   </si>
   <si>
@@ -329,18 +317,6 @@
     <t>Other Service Activities</t>
   </si>
   <si>
-    <t>Net Taxes</t>
-  </si>
-  <si>
-    <t>PRCHG</t>
-  </si>
-  <si>
-    <t>GDP_TYPE</t>
-  </si>
-  <si>
-    <t>GDP type</t>
-  </si>
-  <si>
     <t>CL_GDP_TYPE</t>
   </si>
   <si>
@@ -362,17 +338,71 @@
     <t>Real GDP</t>
   </si>
   <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>Gross Domestic Product</t>
+    <t>NRWGT</t>
+  </si>
+  <si>
+    <t>Norminal GDP weight</t>
+  </si>
+  <si>
+    <t>RLWGT</t>
+  </si>
+  <si>
+    <t>Real GDP weight</t>
+  </si>
+  <si>
+    <t>NRTAX</t>
+  </si>
+  <si>
+    <t>RLTAX</t>
+  </si>
+  <si>
+    <t>Norminal GDP net tax</t>
+  </si>
+  <si>
+    <t>Real GDP net tax</t>
+  </si>
+  <si>
+    <t>TRANSFORMATION</t>
+  </si>
+  <si>
+    <t>Transformation</t>
+  </si>
+  <si>
+    <t>PM1</t>
+  </si>
+  <si>
+    <t>YM1</t>
+  </si>
+  <si>
+    <t>% change over previous period</t>
+  </si>
+  <si>
+    <t>% change over same period last year</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>Estimated value</t>
+  </si>
+  <si>
+    <t>ICLB</t>
+  </si>
+  <si>
+    <t>IC lower bound</t>
+  </si>
+  <si>
+    <t>ICUB</t>
+  </si>
+  <si>
+    <t>IC upper bound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +445,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -437,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -460,6 +496,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,7 +781,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +911,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -889,7 +926,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
@@ -1064,16 +1101,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1086,10 +1121,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1097,7 +1132,39 @@
         <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1107,36 +1174,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2235F8-DCD0-46C4-9C9A-05485E4EEBCB}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
-        <v>103</v>
+        <v>109</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" t="s">
-        <v>106</v>
+        <v>110</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1146,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A81CB80-1365-4A25-8E26-E6A4907DE646}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="122.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1172,127 +1261,127 @@
         <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
@@ -1300,63 +1389,47 @@
         <v>36</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mode codes to the dgp_processing script.
</commit_message>
<xml_diff>
--- a/model/GDP_SDMX_Model.xlsx
+++ b/model/GDP_SDMX_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAP\Fiji\sdd-fbs-data-portal-data-preparation\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E20B9FE-A779-43F8-BFA1-A5AE991CBD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48438F1C-FEDD-4571-9CC9-26326CFCB2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,9 +155,6 @@
     <t>CL_OBS_STATUS</t>
   </si>
   <si>
-    <t>_T</t>
-  </si>
-  <si>
     <t>INDUSTRY_TYPE</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>Other Service Activities</t>
   </si>
   <si>
-    <t>CL_GDP_TYPE</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -338,6 +332,9 @@
     <t>Real GDP</t>
   </si>
   <si>
+    <t>GDP</t>
+  </si>
+  <si>
     <t>NRWGT</t>
   </si>
   <si>
@@ -350,18 +347,6 @@
     <t>Real GDP weight</t>
   </si>
   <si>
-    <t>NRTAX</t>
-  </si>
-  <si>
-    <t>RLTAX</t>
-  </si>
-  <si>
-    <t>Norminal GDP net tax</t>
-  </si>
-  <si>
-    <t>Real GDP net tax</t>
-  </si>
-  <si>
     <t>TRANSFORMATION</t>
   </si>
   <si>
@@ -396,6 +381,21 @@
   </si>
   <si>
     <t>IC upper bound</t>
+  </si>
+  <si>
+    <t>CL_COM_TRANSFORMATION</t>
+  </si>
+  <si>
+    <t>GWA</t>
+  </si>
+  <si>
+    <t>TAX</t>
+  </si>
+  <si>
+    <t>Net Tax</t>
+  </si>
+  <si>
+    <t>Gross Domestic product</t>
   </si>
 </sst>
 </file>
@@ -781,7 +781,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -880,7 +880,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -903,7 +903,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
         <v>36</v>
@@ -911,10 +911,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -926,7 +926,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
@@ -934,10 +934,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -949,7 +949,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
         <v>36</v>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
         <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1018,7 +1018,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -1049,10 +1049,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1101,9 +1101,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1121,50 +1123,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
         <v>101</v>
-      </c>
-      <c r="B5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1182,50 +1168,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1235,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A81CB80-1365-4A25-8E26-E6A4907DE646}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="122.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1258,178 +1244,194 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>72</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>53</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>57</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the codes to process the gdp contributions by industry type
</commit_message>
<xml_diff>
--- a/model/GDP_SDMX_Model.xlsx
+++ b/model/GDP_SDMX_Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAP\Fiji\sdd-fbs-data-portal-data-preparation\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAP\Fiji\latest\sdd-fbs-data-portal-data-preparation\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48438F1C-FEDD-4571-9CC9-26326CFCB2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B3E65E-BD81-4B79-A997-7B5551683B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="121">
   <si>
     <t>Concepts</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>Gross Domestic product</t>
+  </si>
+  <si>
+    <t>RLGDPCNT</t>
+  </si>
+  <si>
+    <t>Real GDP Contribution</t>
   </si>
 </sst>
 </file>
@@ -1101,15 +1107,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1151,6 +1157,14 @@
       </c>
       <c r="B5" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1223,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A81CB80-1365-4A25-8E26-E6A4907DE646}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor changes to the script
</commit_message>
<xml_diff>
--- a/model/GDP_SDMX_Model.xlsx
+++ b/model/GDP_SDMX_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAP\Fiji\latest\sdd-fbs-data-portal-data-preparation\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B3E65E-BD81-4B79-A997-7B5551683B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7540C8EE-6429-4548-871A-AD9FBE006DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSD" sheetId="1" r:id="rId1"/>
@@ -323,9 +323,6 @@
     <t>Norminal GDP</t>
   </si>
   <si>
-    <t>NRGDP</t>
-  </si>
-  <si>
     <t>RLGDP</t>
   </si>
   <si>
@@ -335,9 +332,6 @@
     <t>GDP</t>
   </si>
   <si>
-    <t>NRWGT</t>
-  </si>
-  <si>
     <t>Norminal GDP weight</t>
   </si>
   <si>
@@ -402,6 +396,12 @@
   </si>
   <si>
     <t>Real GDP Contribution</t>
+  </si>
+  <si>
+    <t>NMGDP</t>
+  </si>
+  <si>
+    <t>NMWGT</t>
   </si>
 </sst>
 </file>
@@ -917,10 +917,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -932,7 +932,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6" t="s">
         <v>36</v>
@@ -1109,14 +1109,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>93</v>
@@ -1137,34 +1137,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
         <v>95</v>
-      </c>
-      <c r="B3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1190,42 +1190,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1237,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A81CB80-1365-4A25-8E26-E6A4907DE646}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1258,23 +1258,23 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>69</v>

</xml_diff>